<commit_message>
enhance ContadorApp: add special checkboxes, improve unit selection, and update Excel logging format
</commit_message>
<xml_diff>
--- a/REVs/REV-06-03-2025.xlsx
+++ b/REVs/REV-06-03-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,25 +434,40 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Tiene PT</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Tiene ES</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Tiene IT</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Cantidad Neta</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>UND/ML/GR</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Composición de Lote</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
@@ -461,105 +476,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3666057288104</t>
+          <t>8809844997611</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CLARINS CREMA SOLAR FPS 30</t>
+          <t>Dr.Jart+ | Crema de Manos Hidratante | 100ml</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>No Tiene PT - TRADUZIDO</t>
+          <t>LOTE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Tiene ES</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Tiene IT</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Revisado y Traducido</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3666057288210</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Bruma Solar FPS 50+</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tiene PT</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Tiene ES</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>No Tiene IT - TRADOTTO</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Revisado y Traducido</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>8121669561</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Tiene PT</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Tiene ES</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Tiene IT</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+          <t>12</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>"8809844997611","8809844997611","8809844997611","5245454545545","2323232332323"</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>

</xml_diff>